<commit_message>
issue : http://dev.netforce.com/online/helpdesk-support/issues/285 Tax Audit Report - Add more column
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/tax_audit.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/tax_audit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="198" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>{{#if company_name}}</t>
   </si>
@@ -41,6 +41,15 @@
     <t>Account</t>
   </si>
   <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Tax No.</t>
+  </si>
+  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -60,6 +69,15 @@
   </si>
   <si>
     <t>{{account_name}} ({{account_code}})</t>
+  </si>
+  <si>
+    <t>{{contact_name}}</t>
+  </si>
+  <si>
+    <t>{{number}}</t>
+  </si>
+  <si>
+    <t>{{tax_no}}</t>
   </si>
   <si>
     <t>{{ref}}</t>
@@ -85,36 +103,36 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
-      <name val="Arial"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,7 +144,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -135,47 +153,55 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -185,60 +211,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C15" activeCellId="0" pane="topLeft" sqref="C15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="23.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3450980392157"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.6235294117647"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.0509803921569"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.90980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.3520408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.90816326530612"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5" s="3">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" s="3" customFormat="true" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
@@ -257,53 +296,71 @@
       <c r="F6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="G6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+        <v>21</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="B5:G5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>